<commit_message>
progress on parallel inputs
</commit_message>
<xml_diff>
--- a/pyaez2.1_parvec/function_inputs.xlsx
+++ b/pyaez2.1_parvec/function_inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerrie\Documents\01_LocalCode\repos\PyAEZ\pyaez2.1_parvec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\unfao\pyaez_gaez\repos\PyAEZ_kerrie\PyAEZ\pyaez2.1_parvec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47F97283-E2D7-4E89-A4EC-9DBE764349AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE55DC4-B000-487E-A718-FC5521F55EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11916" yWindow="2796" windowWidth="17280" windowHeight="10044" xr2:uid="{36AB1042-C91C-44F7-BA60-60FD413ED25B}"/>
+    <workbookView xWindow="17805" yWindow="5025" windowWidth="39555" windowHeight="12930" xr2:uid="{36AB1042-C91C-44F7-BA60-60FD413ED25B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>function</t>
   </si>
@@ -59,9 +59,6 @@
     <t>getThermalZone</t>
   </si>
   <si>
-    <t>operates only on monthly means or totals</t>
-  </si>
-  <si>
     <t>operates only on monthly means</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>getLGPEquivalent</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>setParallel</t>
   </si>
   <si>
@@ -125,13 +119,67 @@
     <t>TZoneFallowRequirement</t>
   </si>
   <si>
-    <t>needs output from getThermalZone, operates on monthly and annual aggregates</t>
-  </si>
-  <si>
     <t>needs output from getThermalClimate, getLGP, getLGPEquivalent, getThermalLGP5, AirFrostIndexandPermafrostEvaluation</t>
   </si>
   <si>
     <t>AEZClassification</t>
+  </si>
+  <si>
+    <t>needs function outputs from</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> operates on monthly and annual aggregates</t>
+  </si>
+  <si>
+    <t>needs output from getThermalZone</t>
+  </si>
+  <si>
+    <t>needs daily?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>operates only on monthly means or sums</t>
+  </si>
+  <si>
+    <t>only for acc T during growing</t>
+  </si>
+  <si>
+    <t>only for acc T</t>
+  </si>
+  <si>
+    <t>only for monthly and acc T</t>
+  </si>
+  <si>
+    <t>only for shape and nbytes</t>
+  </si>
+  <si>
+    <t>setDailyClimateData</t>
+  </si>
+  <si>
+    <t>rel_humidity</t>
+  </si>
+  <si>
+    <t>short_rad</t>
+  </si>
+  <si>
+    <t>wind_speed</t>
+  </si>
+  <si>
+    <t>minT_daily</t>
+  </si>
+  <si>
+    <t>carry in memory</t>
+  </si>
+  <si>
+    <t>tclimate</t>
+  </si>
+  <si>
+    <t>output</t>
   </si>
 </sst>
 </file>
@@ -155,12 +203,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -175,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -184,12 +244,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -498,109 +570,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00510AC-DD3E-41AB-98C1-9F98B7065D12}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="6" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5546875" customWidth="1"/>
+    <col min="1" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>2</v>
+      <c r="M2" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="N2" t="s">
         <v>2</v>
@@ -608,68 +685,203 @@
       <c r="O2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>2</v>
       </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="5" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O7" s="3" t="s">
+      <c r="H14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="F8" s="2"/>
+      <c r="P14" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="J15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="J16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>